<commit_message>
Updating (some) RMDs, adding std forms
</commit_message>
<xml_diff>
--- a/form_reporting_templates/Form-1RC_interim.xlsx
+++ b/form_reporting_templates/Form-1RC_interim.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\R libs\workflow\forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\Data dissemination\iotc-reference-forms\form_reporting_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95879ED3-6BC8-4B83-ABCD-C63F7934FCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6A2F2D-E771-47E4-A079-F68DED4C1E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="5O4euoXp3wZfikUhVbwGMfw3acpHwF0QGHqLGhqkSE4QfnoccY7VPEsDDzzEBP5NB49UT+XbcZf1lZQTbDpLFA==" workbookSaltValue="DtEOIJKZ9UKP8oWrD+QpRw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -1421,7 +1421,7 @@
       <c r="D27" s="22"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="+o5eakH6krIsK7d3PB8nk/Eul4T67SgTdhL/FMRuolhTkYYAfYnd2yVTSlzULq5SsGkov/Tgku+9dySl4SSuag==" saltValue="f/LAxS1baHi2CaS4yboKgQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="0h7U1wOmpu2+K04lLxiwBLngxeitul6QXBmvAOai5rnrfvE6hCOecwSOOe2uxiOFYqIPK0tn2HbIVnW+tgq4CQ==" saltValue="8XMNUSoZJLHH3PzbnYBWjg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="4">
     <mergeCell ref="C25:G25"/>
     <mergeCell ref="C8:D8"/>
@@ -2653,7 +2653,7 @@
       <c r="K55" s="55"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="4YamJsHDYbPg7frxG77T0oPG1G9DIZESzB0A6GP9EPWUqRaw2V7gIQzffl2DYKlThR1LIRIDZ/B3/JC5ZeCRvA==" saltValue="v2MWOiGx5Mj6HlWH0aNhLA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="FBUjFu+T4mw0B+piIii5IpWbs28uoLoqTU0wfrTJieqCw4eCLdGIMTOwzBzZyJj8yhsoK0RFexSlGyWF9ml/5A==" saltValue="PU9lHycsAF59HyeUHeTsvQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="5">
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="J4:K4"/>

</xml_diff>